<commit_message>
generated gerbers, added plots and table in ch2
</commit_message>
<xml_diff>
--- a/Elaborato Scritto/data/Misure VCO Tesi.xlsx
+++ b/Elaborato Scritto/data/Misure VCO Tesi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\_PROGETTI\PRJ_SYNTH_MODULES\FG-VCO\Elaborato Scritto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3BAF50-52D6-45B4-A2B7-39D30BD1B36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C236A3-9428-4328-B0FD-B1C62027F934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15210" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Misure VFC110" sheetId="5" r:id="rId1"/>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>I_ref [mA]</t>
-  </si>
-  <si>
-    <t>T_os [us]</t>
   </si>
   <si>
     <t>duty cycle [%]</t>
@@ -185,6 +182,9 @@
   </si>
   <si>
     <t>Vout' [V] formula</t>
+  </si>
+  <si>
+    <t>T_os [ns]</t>
   </si>
 </sst>
 </file>
@@ -430,9 +430,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -444,7 +441,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -463,12 +469,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -640,6 +640,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
@@ -746,6 +749,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>3.9</c:v>
                 </c:pt>
@@ -864,34 +870,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>400.00000000000006</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>800.00000000000011</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1200</c:v>
+                  <c:v>1199.9999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1600.0000000000002</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2000.0000000000002</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2400</c:v>
+                  <c:v>2399.9999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2800.0000000000005</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3200.0000000000005</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3600.0000000000005</c:v>
+                  <c:v>3599.9999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4000.0000000000005</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -969,6 +975,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>342</c:v>
                 </c:pt>
@@ -5846,7 +5855,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5857,7 +5866,8 @@
     <col min="4" max="4" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.7109375" style="5" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="5"/>
+    <col min="7" max="7" width="9.140625" style="5"/>
+    <col min="8" max="8" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="1.7109375" style="5" customWidth="1"/>
     <col min="10" max="11" width="9.140625" style="5"/>
     <col min="12" max="12" width="10" style="5" bestFit="1" customWidth="1"/>
@@ -5883,16 +5893,16 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
       <c r="B2" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="36"/>
       <c r="F2" s="12"/>
       <c r="G2" s="36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H2" s="36"/>
       <c r="I2" s="12"/>
@@ -5906,7 +5916,7 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="22" t="s">
@@ -5924,10 +5934,10 @@
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="24" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" s="24" t="s">
         <v>13</v>
@@ -5955,14 +5965,22 @@
         <v>0</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
       <c r="I5" s="12"/>
       <c r="J5" s="2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="K5" s="2">
         <v>25</v>
@@ -5982,16 +6000,16 @@
         <v>3.9</v>
       </c>
       <c r="E6" s="21">
-        <f t="shared" ref="E6:E15" si="0">(100*B6)/($K$5*$L$5)</f>
+        <f>100*(B6)/($K$5*$L$5)</f>
         <v>4</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="2">
         <v>342</v>
       </c>
-      <c r="H6" s="30">
-        <f t="shared" ref="H6:H15" si="1">(E6/($J$5*10^-6))/1000</f>
-        <v>400.00000000000006</v>
+      <c r="H6" s="35">
+        <f>((E6*10^-2)/($J$5*10^-9)/1000)</f>
+        <v>400</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -6008,17 +6026,17 @@
       <c r="D7" s="2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="E7" s="21">
-        <f t="shared" si="0"/>
+      <c r="E7" s="35">
+        <f t="shared" ref="E7:E15" si="0">100*(B7)/($K$5*$L$5)</f>
         <v>8</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="2">
         <v>805</v>
       </c>
-      <c r="H7" s="30">
-        <f t="shared" si="1"/>
-        <v>800.00000000000011</v>
+      <c r="H7" s="35">
+        <f>((E7*10^-2)/($J$5*10^-9)/1000)</f>
+        <v>800</v>
       </c>
       <c r="I7" s="12"/>
       <c r="M7" s="19"/>
@@ -6032,7 +6050,7 @@
       <c r="D8" s="2">
         <v>13.6</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="35">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -6040,9 +6058,9 @@
       <c r="G8" s="2">
         <v>1192</v>
       </c>
-      <c r="H8" s="30">
-        <f t="shared" si="1"/>
-        <v>1200</v>
+      <c r="H8" s="35">
+        <f t="shared" ref="H8:H15" si="1">((E8*10^-2)/($J$5*10^-9)/1000)</f>
+        <v>1199.9999999999998</v>
       </c>
       <c r="I8" s="12"/>
       <c r="M8" s="19"/>
@@ -6056,7 +6074,7 @@
       <c r="D9" s="2">
         <v>17.989999999999998</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="35">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -6064,9 +6082,9 @@
       <c r="G9" s="2">
         <v>1580</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="35">
         <f t="shared" si="1"/>
-        <v>1600.0000000000002</v>
+        <v>1600</v>
       </c>
       <c r="I9" s="12"/>
       <c r="M9" s="19"/>
@@ -6080,7 +6098,7 @@
       <c r="D10" s="2">
         <v>22.4</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="35">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -6088,9 +6106,9 @@
       <c r="G10" s="2">
         <v>1978</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="35">
         <f t="shared" si="1"/>
-        <v>2000.0000000000002</v>
+        <v>2000</v>
       </c>
       <c r="I10" s="12"/>
       <c r="M10" s="19"/>
@@ -6104,7 +6122,7 @@
       <c r="D11" s="2">
         <v>26.83</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="35">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -6112,9 +6130,9 @@
       <c r="G11" s="2">
         <v>2377</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="35">
         <f t="shared" si="1"/>
-        <v>2400</v>
+        <v>2399.9999999999995</v>
       </c>
       <c r="I11" s="12"/>
       <c r="M11" s="19"/>
@@ -6128,7 +6146,7 @@
       <c r="D12" s="2">
         <v>31.38</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="35">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -6136,9 +6154,9 @@
       <c r="G12" s="2">
         <v>2776</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="35">
         <f t="shared" si="1"/>
-        <v>2800.0000000000005</v>
+        <v>2800</v>
       </c>
       <c r="I12" s="12"/>
       <c r="M12" s="19"/>
@@ -6152,7 +6170,7 @@
       <c r="D13" s="2">
         <v>35.549999999999997</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="35">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -6160,9 +6178,9 @@
       <c r="G13" s="2">
         <v>3165</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="35">
         <f t="shared" si="1"/>
-        <v>3200.0000000000005</v>
+        <v>3200</v>
       </c>
       <c r="I13" s="12"/>
       <c r="M13" s="19"/>
@@ -6176,7 +6194,7 @@
       <c r="D14" s="2">
         <v>40.119999999999997</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="35">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
@@ -6184,9 +6202,9 @@
       <c r="G14" s="2">
         <v>3568</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="35">
         <f t="shared" si="1"/>
-        <v>3600.0000000000005</v>
+        <v>3599.9999999999995</v>
       </c>
       <c r="I14" s="12"/>
       <c r="M14" s="19"/>
@@ -6200,7 +6218,7 @@
       <c r="D15" s="2">
         <v>44.23</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="35">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -6208,9 +6226,9 @@
       <c r="G15" s="2">
         <v>3883</v>
       </c>
-      <c r="H15" s="30">
+      <c r="H15" s="35">
         <f t="shared" si="1"/>
-        <v>4000.0000000000005</v>
+        <v>4000</v>
       </c>
       <c r="I15" s="12"/>
       <c r="M15" s="19"/>
@@ -6522,7 +6540,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>2</v>
@@ -6535,7 +6553,7 @@
         <v>7</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>2</v>
@@ -6548,7 +6566,7 @@
         <v>7</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>2</v>
@@ -6561,7 +6579,7 @@
         <v>7</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U2" s="8" t="s">
         <v>2</v>
@@ -6580,25 +6598,25 @@
         <v>4</v>
       </c>
       <c r="C3" s="13"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
       <c r="H3" s="13"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
       <c r="M3" s="13"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
       <c r="R3" s="12"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
       <c r="W3" s="14"/>
       <c r="X3" s="10"/>
       <c r="Y3" s="10"/>
@@ -6610,25 +6628,25 @@
         <v>0</v>
       </c>
       <c r="C4" s="13"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
       <c r="M4" s="13"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
       <c r="R4" s="12"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="44"/>
-      <c r="U4" s="44"/>
-      <c r="V4" s="44"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
       <c r="W4" s="14"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -6637,25 +6655,25 @@
         <v>1</v>
       </c>
       <c r="C5" s="13"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
       <c r="M5" s="13"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
       <c r="R5" s="12"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="V5" s="44"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
       <c r="W5" s="14"/>
     </row>
     <row r="6" spans="1:28" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
@@ -7157,7 +7175,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>2</v>
@@ -7173,10 +7191,10 @@
         <v>4</v>
       </c>
       <c r="C20" s="13"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="41"/>
       <c r="H20" s="13"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
@@ -7202,10 +7220,10 @@
         <v>0</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="44"/>
       <c r="H21" s="13"/>
       <c r="I21" s="7"/>
       <c r="J21" s="10"/>
@@ -7231,10 +7249,10 @@
         <v>1</v>
       </c>
       <c r="C22" s="13"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="44"/>
       <c r="H22" s="13"/>
       <c r="I22" s="7"/>
       <c r="J22" s="10"/>
@@ -7250,9 +7268,9 @@
       <c r="T22" s="10"/>
       <c r="U22" s="10"/>
       <c r="V22" s="10"/>
-      <c r="X22" s="31"/>
-      <c r="Y22" s="31"/>
-      <c r="Z22" s="31"/>
+      <c r="X22" s="30"/>
+      <c r="Y22" s="30"/>
+      <c r="Z22" s="30"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
@@ -8012,6 +8030,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D20:G20"/>
     <mergeCell ref="S3:V3"/>
     <mergeCell ref="S4:V4"/>
     <mergeCell ref="S5:V5"/>
@@ -8021,12 +8045,6 @@
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N5:Q5"/>
     <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -8074,47 +8092,47 @@
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="45"/>
       <c r="F2" s="12"/>
       <c r="G2" s="45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="45"/>
       <c r="I2" s="12"/>
       <c r="L2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="I3" s="12"/>
       <c r="K3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="O3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
@@ -8151,7 +8169,7 @@
         <v>-6.7</v>
       </c>
       <c r="I5" s="12"/>
-      <c r="K5" s="32">
+      <c r="K5" s="31">
         <v>-6</v>
       </c>
       <c r="L5" s="5">
@@ -8174,7 +8192,7 @@
       <c r="D6" s="5">
         <v>-5.08</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="31">
         <f t="shared" ref="E6:E19" si="0">B6</f>
         <v>-5</v>
       </c>
@@ -8182,18 +8200,18 @@
       <c r="G6" s="5">
         <v>-5.7670000000000003</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="31">
         <f t="shared" ref="H6:H19" si="1">B6-0.7</f>
         <v>-5.7</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="K6" s="32">
+      <c r="K6" s="31">
         <v>-5</v>
       </c>
       <c r="L6" s="5">
         <v>0.113</v>
       </c>
-      <c r="M6" s="32">
+      <c r="M6" s="31">
         <f t="shared" ref="M6:M17" si="2">(K6+$O$5)*(-0.02)</f>
         <v>9.0120000000000006E-2</v>
       </c>
@@ -8207,7 +8225,7 @@
       <c r="D7" s="5">
         <v>-4.0069999999999997</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="31">
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
@@ -8215,18 +8233,18 @@
       <c r="G7" s="5">
         <v>-4.7530000000000001</v>
       </c>
-      <c r="H7" s="32">
+      <c r="H7" s="31">
         <f t="shared" si="1"/>
         <v>-4.7</v>
       </c>
       <c r="I7" s="12"/>
-      <c r="K7" s="32">
+      <c r="K7" s="31">
         <v>-4</v>
       </c>
       <c r="L7" s="5">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="M7" s="32">
+      <c r="M7" s="31">
         <f t="shared" si="2"/>
         <v>7.0120000000000002E-2</v>
       </c>
@@ -8240,7 +8258,7 @@
       <c r="D8" s="5">
         <v>-3.0070000000000001</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
@@ -8248,18 +8266,18 @@
       <c r="G8" s="5">
         <v>-3.7349999999999999</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="31">
         <f t="shared" si="1"/>
         <v>-3.7</v>
       </c>
       <c r="I8" s="12"/>
-      <c r="K8" s="32">
+      <c r="K8" s="31">
         <v>-3</v>
       </c>
       <c r="L8" s="5">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="M8" s="32">
+      <c r="M8" s="31">
         <f t="shared" si="2"/>
         <v>5.0120000000000005E-2</v>
       </c>
@@ -8273,7 +8291,7 @@
       <c r="D9" s="5">
         <v>-2.0059999999999998</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="31">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
@@ -8281,18 +8299,18 @@
       <c r="G9" s="5">
         <v>-2.71</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="31">
         <f t="shared" si="1"/>
         <v>-2.7</v>
       </c>
       <c r="I9" s="12"/>
-      <c r="K9" s="32">
+      <c r="K9" s="31">
         <v>-2</v>
       </c>
       <c r="L9" s="5">
         <v>5.5E-2</v>
       </c>
-      <c r="M9" s="32">
+      <c r="M9" s="31">
         <f t="shared" si="2"/>
         <v>3.0120000000000001E-2</v>
       </c>
@@ -8306,7 +8324,7 @@
       <c r="D10" s="5">
         <v>-1.0049999999999999</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
@@ -8314,18 +8332,18 @@
       <c r="G10" s="5">
         <v>-1.671</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="31">
         <f t="shared" si="1"/>
         <v>-1.7</v>
       </c>
       <c r="I10" s="12"/>
-      <c r="K10" s="32">
+      <c r="K10" s="31">
         <v>-1</v>
       </c>
       <c r="L10" s="5">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="M10" s="32">
+      <c r="M10" s="31">
         <f t="shared" si="2"/>
         <v>1.0120000000000001E-2</v>
       </c>
@@ -8339,7 +8357,7 @@
       <c r="D11" s="5">
         <v>-0.90500000000000003</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="31">
         <f t="shared" si="0"/>
         <v>-0.9</v>
       </c>
@@ -8347,18 +8365,18 @@
       <c r="G11" s="5">
         <v>-1.5660000000000001</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="31">
         <f t="shared" si="1"/>
         <v>-1.6</v>
       </c>
       <c r="I11" s="12"/>
-      <c r="K11" s="32">
+      <c r="K11" s="31">
         <v>0</v>
       </c>
       <c r="L11" s="5">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="M11" s="32">
+      <c r="M11" s="31">
         <f t="shared" si="2"/>
         <v>-9.8799999999999999E-3</v>
       </c>
@@ -8372,7 +8390,7 @@
       <c r="D12" s="5">
         <v>-0.80400000000000005</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <f t="shared" si="0"/>
         <v>-0.8</v>
       </c>
@@ -8380,18 +8398,18 @@
       <c r="G12" s="5">
         <v>-1.46</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="31">
         <f t="shared" si="1"/>
         <v>-1.5</v>
       </c>
       <c r="I12" s="12"/>
-      <c r="K12" s="32">
+      <c r="K12" s="31">
         <v>1</v>
       </c>
       <c r="L12" s="5">
         <v>-2.4E-2</v>
       </c>
-      <c r="M12" s="32">
+      <c r="M12" s="31">
         <f t="shared" si="2"/>
         <v>-2.988E-2</v>
       </c>
@@ -8405,7 +8423,7 @@
       <c r="D13" s="5">
         <v>-0.70399999999999996</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="31">
         <f t="shared" si="0"/>
         <v>-0.7</v>
       </c>
@@ -8413,18 +8431,18 @@
       <c r="G13" s="5">
         <v>-1.353</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="31">
         <f t="shared" si="1"/>
         <v>-1.4</v>
       </c>
       <c r="I13" s="12"/>
-      <c r="K13" s="32">
+      <c r="K13" s="31">
         <v>2</v>
       </c>
       <c r="L13" s="5">
         <v>-4.3999999999999997E-2</v>
       </c>
-      <c r="M13" s="32">
+      <c r="M13" s="31">
         <f t="shared" si="2"/>
         <v>-4.9879999999999994E-2</v>
       </c>
@@ -8438,7 +8456,7 @@
       <c r="D14" s="5">
         <v>-0.60399999999999998</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="31">
         <f t="shared" si="0"/>
         <v>-0.6</v>
       </c>
@@ -8446,18 +8464,18 @@
       <c r="G14" s="5">
         <v>-1.2450000000000001</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="31">
         <f t="shared" si="1"/>
         <v>-1.2999999999999998</v>
       </c>
       <c r="I14" s="12"/>
-      <c r="K14" s="32">
+      <c r="K14" s="31">
         <v>3</v>
       </c>
       <c r="L14" s="5">
         <v>-6.4000000000000001E-2</v>
       </c>
-      <c r="M14" s="32">
+      <c r="M14" s="31">
         <f t="shared" si="2"/>
         <v>-6.9879999999999998E-2</v>
       </c>
@@ -8471,7 +8489,7 @@
       <c r="D15" s="5">
         <v>-0.504</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="31">
         <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
@@ -8479,18 +8497,18 @@
       <c r="G15" s="5">
         <v>-1.135</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="31">
         <f t="shared" si="1"/>
         <v>-1.2</v>
       </c>
       <c r="I15" s="12"/>
-      <c r="K15" s="32">
+      <c r="K15" s="31">
         <v>4</v>
       </c>
       <c r="L15" s="5">
         <v>-8.3000000000000004E-2</v>
       </c>
-      <c r="M15" s="32">
+      <c r="M15" s="31">
         <f t="shared" si="2"/>
         <v>-8.9880000000000002E-2</v>
       </c>
@@ -8504,7 +8522,7 @@
       <c r="D16" s="5">
         <v>-0.40400000000000003</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="31">
         <f t="shared" si="0"/>
         <v>-0.4</v>
       </c>
@@ -8512,18 +8530,18 @@
       <c r="G16" s="5">
         <v>-1.0229999999999999</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="31">
         <f t="shared" si="1"/>
         <v>-1.1000000000000001</v>
       </c>
       <c r="I16" s="12"/>
-      <c r="K16" s="32">
+      <c r="K16" s="31">
         <v>5</v>
       </c>
       <c r="L16" s="5">
         <v>-0.10299999999999999</v>
       </c>
-      <c r="M16" s="32">
+      <c r="M16" s="31">
         <f t="shared" si="2"/>
         <v>-0.10987999999999999</v>
       </c>
@@ -8537,7 +8555,7 @@
       <c r="D17" s="5">
         <v>-0.30399999999999999</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="31">
         <f t="shared" si="0"/>
         <v>-0.3</v>
       </c>
@@ -8545,18 +8563,18 @@
       <c r="G17" s="5">
         <v>-0.90900000000000003</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="31">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="I17" s="12"/>
-      <c r="K17" s="32">
+      <c r="K17" s="31">
         <v>6</v>
       </c>
       <c r="L17" s="5">
         <v>-0.122</v>
       </c>
-      <c r="M17" s="32">
+      <c r="M17" s="31">
         <f t="shared" si="2"/>
         <v>-0.12988</v>
       </c>
@@ -8570,7 +8588,7 @@
       <c r="D18" s="5">
         <v>-0.20399999999999999</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="31">
         <f t="shared" si="0"/>
         <v>-0.2</v>
       </c>
@@ -8578,7 +8596,7 @@
       <c r="G18" s="5">
         <v>-0.78900000000000003</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="31">
         <f t="shared" si="1"/>
         <v>-0.89999999999999991</v>
       </c>
@@ -8593,7 +8611,7 @@
       <c r="D19" s="5">
         <v>-0.10299999999999999</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="31">
         <f t="shared" si="0"/>
         <v>-0.1</v>
       </c>
@@ -8601,7 +8619,7 @@
       <c r="G19" s="5">
         <v>-0.65400000000000003</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="31">
         <f t="shared" si="1"/>
         <v>-0.79999999999999993</v>
       </c>
@@ -8616,7 +8634,7 @@
       <c r="D20" s="5">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="31">
         <v>0</v>
       </c>
       <c r="F20" s="12"/>
@@ -8634,17 +8652,17 @@
         <v>0.1</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="32">
+      <c r="D21" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="31">
         <v>0</v>
       </c>
       <c r="F21" s="12"/>
-      <c r="G21" s="32">
+      <c r="G21" s="31">
         <v>8.64</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="31">
         <v>12</v>
       </c>
       <c r="I21" s="12"/>
@@ -8655,17 +8673,17 @@
         <v>0.2</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="32">
+      <c r="D22" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="31">
         <v>0</v>
       </c>
       <c r="F22" s="12"/>
-      <c r="G22" s="32">
+      <c r="G22" s="31">
         <v>8.64</v>
       </c>
-      <c r="H22" s="32">
+      <c r="H22" s="31">
         <v>12</v>
       </c>
       <c r="I22" s="12"/>
@@ -8676,17 +8694,17 @@
         <v>0.3</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="32">
+      <c r="D23" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="31">
         <v>0</v>
       </c>
       <c r="F23" s="12"/>
-      <c r="G23" s="32">
+      <c r="G23" s="31">
         <v>8.64</v>
       </c>
-      <c r="H23" s="35">
+      <c r="H23" s="34">
         <v>12</v>
       </c>
       <c r="I23" s="12"/>
@@ -8697,17 +8715,17 @@
         <v>0.4</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="32">
+      <c r="D24" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="31">
         <v>0</v>
       </c>
       <c r="F24" s="12"/>
-      <c r="G24" s="32">
+      <c r="G24" s="31">
         <v>8.64</v>
       </c>
-      <c r="H24" s="35">
+      <c r="H24" s="34">
         <v>12</v>
       </c>
       <c r="I24" s="12"/>
@@ -8718,17 +8736,17 @@
         <v>0.5</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="32">
+      <c r="D25" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="31">
         <v>0</v>
       </c>
       <c r="F25" s="12"/>
-      <c r="G25" s="32">
+      <c r="G25" s="31">
         <v>8.64</v>
       </c>
-      <c r="H25" s="35">
+      <c r="H25" s="34">
         <v>12</v>
       </c>
       <c r="I25" s="12"/>
@@ -8739,17 +8757,17 @@
         <v>0.6</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="32">
+      <c r="D26" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="31">
         <v>0</v>
       </c>
       <c r="F26" s="12"/>
-      <c r="G26" s="32">
+      <c r="G26" s="31">
         <v>8.64</v>
       </c>
-      <c r="H26" s="35">
+      <c r="H26" s="34">
         <v>12</v>
       </c>
       <c r="I26" s="12"/>
@@ -8760,17 +8778,17 @@
         <v>0.7</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="32">
+      <c r="D27" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="31">
         <v>0</v>
       </c>
       <c r="F27" s="12"/>
-      <c r="G27" s="32">
+      <c r="G27" s="31">
         <v>8.64</v>
       </c>
-      <c r="H27" s="35">
+      <c r="H27" s="34">
         <v>12</v>
       </c>
       <c r="I27" s="12"/>
@@ -8781,17 +8799,17 @@
         <v>0.8</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="32">
+      <c r="D28" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="31">
         <v>0</v>
       </c>
       <c r="F28" s="12"/>
-      <c r="G28" s="32">
+      <c r="G28" s="31">
         <v>8.64</v>
       </c>
-      <c r="H28" s="35">
+      <c r="H28" s="34">
         <v>12</v>
       </c>
       <c r="I28" s="12"/>
@@ -8802,17 +8820,17 @@
         <v>0.9</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="32">
+      <c r="D29" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="31">
         <v>0</v>
       </c>
       <c r="F29" s="12"/>
-      <c r="G29" s="32">
+      <c r="G29" s="31">
         <v>8.64</v>
       </c>
-      <c r="H29" s="35">
+      <c r="H29" s="34">
         <v>12</v>
       </c>
       <c r="I29" s="12"/>
@@ -8823,17 +8841,17 @@
         <v>1</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="32">
+      <c r="D30" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="31">
         <v>0</v>
       </c>
       <c r="F30" s="12"/>
-      <c r="G30" s="32">
+      <c r="G30" s="31">
         <v>8.64</v>
       </c>
-      <c r="H30" s="35">
+      <c r="H30" s="34">
         <v>12</v>
       </c>
       <c r="I30" s="12"/>
@@ -8844,17 +8862,17 @@
         <v>2</v>
       </c>
       <c r="C31" s="12"/>
-      <c r="D31" s="32">
+      <c r="D31" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="31">
         <v>0</v>
       </c>
       <c r="F31" s="12"/>
-      <c r="G31" s="32">
+      <c r="G31" s="31">
         <v>8.64</v>
       </c>
-      <c r="H31" s="35">
+      <c r="H31" s="34">
         <v>12</v>
       </c>
       <c r="I31" s="12"/>
@@ -8865,17 +8883,17 @@
         <v>3</v>
       </c>
       <c r="C32" s="12"/>
-      <c r="D32" s="32">
+      <c r="D32" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="31">
         <v>0</v>
       </c>
       <c r="F32" s="12"/>
-      <c r="G32" s="32">
+      <c r="G32" s="31">
         <v>8.64</v>
       </c>
-      <c r="H32" s="35">
+      <c r="H32" s="34">
         <v>12</v>
       </c>
       <c r="I32" s="12"/>
@@ -8886,17 +8904,17 @@
         <v>4</v>
       </c>
       <c r="C33" s="12"/>
-      <c r="D33" s="32">
+      <c r="D33" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="31">
         <v>0</v>
       </c>
       <c r="F33" s="12"/>
-      <c r="G33" s="32">
+      <c r="G33" s="31">
         <v>8.64</v>
       </c>
-      <c r="H33" s="35">
+      <c r="H33" s="34">
         <v>12</v>
       </c>
       <c r="I33" s="12"/>
@@ -8907,17 +8925,17 @@
         <v>5</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="32">
+      <c r="D34" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="31">
         <v>0</v>
       </c>
       <c r="F34" s="12"/>
-      <c r="G34" s="32">
+      <c r="G34" s="31">
         <v>8.64</v>
       </c>
-      <c r="H34" s="35">
+      <c r="H34" s="34">
         <v>12</v>
       </c>
       <c r="I34" s="12"/>
@@ -8928,17 +8946,17 @@
         <v>6</v>
       </c>
       <c r="C35" s="12"/>
-      <c r="D35" s="32">
+      <c r="D35" s="31">
         <v>7.4200000000000004E-3</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="31">
         <v>0</v>
       </c>
       <c r="F35" s="12"/>
-      <c r="G35" s="32">
+      <c r="G35" s="31">
         <v>8.64</v>
       </c>
-      <c r="H35" s="35">
+      <c r="H35" s="34">
         <v>12</v>
       </c>
       <c r="I35" s="12"/>
@@ -8983,7 +9001,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
@@ -9039,37 +9057,37 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
     </row>
@@ -9097,13 +9115,13 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -9205,208 +9223,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
+      <c r="A1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
     </row>
     <row r="3" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
     </row>
     <row r="5" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
     </row>
     <row r="12" spans="1:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L15" s="17"/>
@@ -9437,7 +9455,7 @@
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="20"/>
       <c r="C2" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>
@@ -9445,7 +9463,7 @@
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="22"/>
       <c r="C3" s="46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
@@ -9453,7 +9471,7 @@
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="23"/>
       <c r="C4" s="46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="46"/>
       <c r="E4" s="46"/>
@@ -9461,7 +9479,7 @@
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="24"/>
       <c r="C5" s="46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="46"/>
       <c r="E5" s="46"/>
@@ -9469,7 +9487,7 @@
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="25"/>
       <c r="C6" s="46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="46"/>
       <c r="E6" s="46"/>

</xml_diff>

<commit_message>
refined to chapter 4
</commit_message>
<xml_diff>
--- a/Elaborato Scritto/data/Misure VCO Tesi.xlsx
+++ b/Elaborato Scritto/data/Misure VCO Tesi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\_PROGETTI\PRJ_SYNTH_MODULES\FG-VCO\Elaborato Scritto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631F9F74-D267-4288-9CDC-5BC84D852DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53390812-45E0-4302-A879-A7AA49EBDC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-690" yWindow="795" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Misure VFC110" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>Vin [V]</t>
   </si>
@@ -213,6 +213,15 @@
   <si>
     <t>Vd</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A dB calcolato</t>
+  </si>
+  <si>
+    <t>A dB misurato</t>
+  </si>
 </sst>
 </file>
 
@@ -220,7 +229,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -341,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -461,6 +470,21 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -468,12 +492,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4267,6 +4285,497 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Misure Stadio di Uscita'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A dB calcolato</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Misure Stadio di Uscita'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>512000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Misure Stadio di Uscita'!$G$4:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>-5.917752955845818E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.3670528022348052E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-9.4674372327238328E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.7857372056880638E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.5123188882178356E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-6.0179324114907472E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.23587008228984918</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.87515945393713102</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.7715247749318932</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6.6010930803660717</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-11.843543659922357</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-17.645685382570811</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-23.609909488085265</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-29.410531667261782</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-35.427399259349919</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9DCA-4A86-BF8E-51030704565F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Misure Stadio di Uscita'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A dB misurato</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Misure Stadio di Uscita'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>512000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Misure Stadio di Uscita'!$F$4:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.124086248</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.124086248</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.124086248</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.97697135099999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3.320880812</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-7.582076357</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-13.04578929</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-18.687505290000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-23.429910150000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-27.866885140000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-28.336507059999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9DCA-4A86-BF8E-51030704565F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1741653024"/>
+        <c:axId val="1741654688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1741653024"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1741654688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1741654688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1741653024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -5186,10 +5695,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>7.64</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.0399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9</c:v>
@@ -5207,40 +5716,40 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>3.8199999999999998E-2</c:v>
+                  <c:v>5.2299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.6399999999999996E-2</c:v>
+                  <c:v>0.1046</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15279999999999999</c:v>
+                  <c:v>0.2092</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.30559999999999998</c:v>
+                  <c:v>0.41839999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.61119999999999997</c:v>
+                  <c:v>0.83679999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2223999999999999</c:v>
+                  <c:v>1.6736</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4447999999999999</c:v>
+                  <c:v>3.3472</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.8895999999999997</c:v>
+                  <c:v>6.6943999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.7791999999999994</c:v>
+                  <c:v>10.432078724158499</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.054130733634997</c:v>
+                  <c:v>13.3888</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.558399999999999</c:v>
+                  <c:v>26.7776</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>39.116799999999998</c:v>
+                  <c:v>53.555199999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5309,10 +5818,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>7.64</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.0399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9</c:v>
@@ -5330,40 +5839,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>3.8199999999999998E-2</c:v>
+                  <c:v>5.2299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.1000000000000003E-2</c:v>
+                  <c:v>9.9900000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17</c:v>
+                  <c:v>0.20300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35399999999999998</c:v>
+                  <c:v>0.41299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.71699999999999997</c:v>
+                  <c:v>0.82699999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4550000000000001</c:v>
+                  <c:v>1.6779999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.89</c:v>
+                  <c:v>3.37</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.48</c:v>
+                  <c:v>6.81</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.24</c:v>
+                  <c:v>10.45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.33</c:v>
+                  <c:v>10.45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.38</c:v>
+                  <c:v>10.45</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.39</c:v>
+                  <c:v>10.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5372,6 +5881,129 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-CE80-4451-B611-965AF1D27A59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Misure VCO'!$Q$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vattesa[V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Misure VCO'!$P$6:$P$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Misure VCO'!$U$6:$U$17</c:f>
+              <c:numCache>
+                <c:formatCode>0,000</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3.9600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9133540430338614E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15813427325858678</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.31600315420026737</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63147596916720683</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2618921499212232</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5216665016292414</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0391009610734425</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.8483601235209406</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.069744940294523</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.122590109999848</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40.211409041232486</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-61EF-44EE-85A9-61CF99714A26}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7004,10 +7636,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>7.64</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.0399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9</c:v>
@@ -7025,40 +7657,40 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.91151515151515161</c:v>
+                  <c:v>0.99696969696969706</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0272727272727273</c:v>
+                  <c:v>1.1554545454545455</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2587878787878788</c:v>
+                  <c:v>1.4392424242424244</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4641818181818183</c:v>
+                  <c:v>1.5026363636363638</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5567878787878788</c:v>
+                  <c:v>1.6294242424242427</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.742</c:v>
+                  <c:v>1.883</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.1124242424242423</c:v>
+                  <c:v>2.3901515151515151</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8532727272727274</c:v>
+                  <c:v>3.4044545454545458</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.3349696969696971</c:v>
+                  <c:v>4.5370844618662121</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.4182820404954537</c:v>
+                  <c:v>5.4330606060606055</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.2983636363636357</c:v>
+                  <c:v>9.4902727272727265</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.225151515151516</c:v>
+                  <c:v>17.60469696969697</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7127,10 +7759,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>7.64</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.0399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9</c:v>
@@ -7145,43 +7777,43 @@
             <c:numRef>
               <c:f>'Misure VCO'!$U$6:$U$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.78600000000000003</c:v>
+                  <c:v>3.9600000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.93600000000000005</c:v>
+                  <c:v>7.9133540430338614E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.131</c:v>
+                  <c:v>0.15813427325858678</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2529999999999999</c:v>
+                  <c:v>0.31600315420026737</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4139999999999999</c:v>
+                  <c:v>0.63147596916720683</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7050000000000001</c:v>
+                  <c:v>1.2618921499212232</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.21</c:v>
+                  <c:v>2.5216665016292414</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.12</c:v>
+                  <c:v>5.0391009610734425</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.63</c:v>
+                  <c:v>7.8483601235209406</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.68</c:v>
+                  <c:v>10.069744940294523</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.62</c:v>
+                  <c:v>20.122590109999848</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.74</c:v>
+                  <c:v>40.211409041232486</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8075,6 +8707,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -10976,6 +11648,522 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16140,6 +17328,47 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>80961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{280C0082-0836-EE42-EFA8-C2B9505A6E4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
@@ -16539,21 +17768,21 @@
         <v>8</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="43"/>
+      <c r="E2" s="48"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="43"/>
+      <c r="H2" s="48"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="43" t="s">
+      <c r="J2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
       <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -17115,10 +18344,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AK60"/>
+  <dimension ref="A1:AK76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X57" sqref="X57"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17366,7 +18595,7 @@
       <c r="AI3" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="AK3" s="46" t="s">
+      <c r="AK3" s="44" t="s">
         <v>42</v>
       </c>
     </row>
@@ -17474,7 +18703,7 @@
         <v>2.3636363636363636E-2</v>
       </c>
       <c r="F6" s="42">
-        <f>IF(E6&lt;($AK$4/(D$1)),(E$6+E6)*D$1,(E$6+E6)*G$1+$AK$4)+$AK$4</f>
+        <f t="shared" ref="F6:F17" si="0">IF(E6&lt;($AK$4/(D$1)),(E$6+E6)*D$1,(E$6+E6)*G$1+$AK$4)+$AK$4</f>
         <v>1.1527272727272728</v>
       </c>
       <c r="G6" s="32">
@@ -17508,21 +18737,22 @@
       </c>
       <c r="Q6" s="32">
         <f>R6</f>
-        <v>3.8199999999999998E-2</v>
+        <v>5.2299999999999999E-2</v>
       </c>
       <c r="R6" s="36">
-        <v>3.8199999999999998E-2</v>
+        <v>5.2299999999999999E-2</v>
       </c>
       <c r="S6" s="42">
         <f>(Q$6+Q6)/3.3</f>
-        <v>2.3151515151515152E-2</v>
+        <v>3.1696969696969696E-2</v>
       </c>
       <c r="T6" s="42">
         <f>IF(S6&lt;$AK$4/(R$1),S6*R$1,S6*U$1+$AK$4)+$AK$4</f>
-        <v>0.91151515151515161</v>
-      </c>
-      <c r="U6" s="32">
-        <v>0.78600000000000003</v>
+        <v>0.99696969696969706</v>
+      </c>
+      <c r="U6" s="38">
+        <f>(12*3300/1000000)*EXP(0.018*P6/0.026)</f>
+        <v>3.9600000000000003E-2</v>
       </c>
       <c r="V6" s="37"/>
       <c r="W6" s="33">
@@ -17582,11 +18812,11 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="E7" s="42">
-        <f t="shared" ref="E7:E17" si="0">(C$6+C7)/3.3</f>
+        <f t="shared" ref="E7:E17" si="1">(C$6+C7)/3.3</f>
         <v>3.5454545454545454E-2</v>
       </c>
       <c r="F7" s="42">
-        <f>IF(E7&lt;($AK$4/(D$1)),(E$6+E7)*D$1,(E$6+E7)*G$1+$AK$4)+$AK$4</f>
+        <f t="shared" si="0"/>
         <v>1.270909090909091</v>
       </c>
       <c r="G7" s="32">
@@ -17604,11 +18834,11 @@
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="L7" s="42">
-        <f t="shared" ref="L7:L17" si="1">(J$6+J7)/3.3</f>
+        <f t="shared" ref="L7:L17" si="2">(J$6+J7)/3.3</f>
         <v>4.1818181818181824E-2</v>
       </c>
       <c r="M7" s="42">
-        <f t="shared" ref="M7:M17" si="2">IF(L7&lt;($AK$4/(K$1)),L7*K$1,L7*G$1+$AK$4)+$AK$4</f>
+        <f t="shared" ref="M7:M17" si="3">IF(L7&lt;($AK$4/(K$1)),L7*K$1,L7*G$1+$AK$4)+$AK$4</f>
         <v>0.81800000000000006</v>
       </c>
       <c r="N7" s="32">
@@ -17620,21 +18850,22 @@
       </c>
       <c r="Q7" s="38">
         <f>Q$6*2^P7</f>
-        <v>7.6399999999999996E-2</v>
+        <v>0.1046</v>
       </c>
       <c r="R7" s="36">
-        <v>8.1000000000000003E-2</v>
+        <v>9.9900000000000003E-2</v>
       </c>
       <c r="S7" s="42">
-        <f t="shared" ref="S7:S17" si="3">(Q$6+Q7)/3.3</f>
-        <v>3.4727272727272725E-2</v>
+        <f t="shared" ref="S7:S17" si="4">(Q$6+Q7)/3.3</f>
+        <v>4.7545454545454544E-2</v>
       </c>
       <c r="T7" s="42">
-        <f t="shared" ref="T7:T17" si="4">IF(S7&lt;$AK$4/(R$1),S7*R$1,S7*U$1+$AK$4)+$AK$4</f>
-        <v>1.0272727272727273</v>
-      </c>
-      <c r="U7" s="32">
-        <v>0.93600000000000005</v>
+        <f t="shared" ref="T7:T17" si="5">IF(S7&lt;$AK$4/(R$1),S7*R$1,S7*U$1+$AK$4)+$AK$4</f>
+        <v>1.1554545454545455</v>
+      </c>
+      <c r="U7" s="38">
+        <f t="shared" ref="U7:U17" si="6">(12*3300/1000000)*EXP(0.018*P7/0.026)</f>
+        <v>7.9133540430338614E-2</v>
       </c>
       <c r="V7" s="37"/>
       <c r="W7" s="33">
@@ -17648,11 +18879,11 @@
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="Z7" s="42">
-        <f t="shared" ref="Z7:Z17" si="5">(X$6+X7)/3.3</f>
+        <f t="shared" ref="Z7:Z17" si="7">(X$6+X7)/3.3</f>
         <v>3.4545454545454546E-2</v>
       </c>
       <c r="AA7" s="42">
-        <f t="shared" ref="AA7:AA17" si="6">Z7*Y$1+$AK$4</f>
+        <f t="shared" ref="AA7:AA17" si="8">Z7*Y$1+$AK$4</f>
         <v>0.79400000000000004</v>
       </c>
       <c r="AB7" s="33">
@@ -17670,11 +18901,11 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="AG7" s="42">
-        <f t="shared" ref="AG7:AG17" si="7">(AE$6+AE7)/3.3</f>
+        <f t="shared" ref="AG7:AG17" si="9">(AE$6+AE7)/3.3</f>
         <v>3.4545454545454546E-2</v>
       </c>
       <c r="AH7" s="42">
-        <f t="shared" ref="AH7:AH17" si="8">IF(AG7&lt;$AK$4/(AF$1),AG7*AF$1,(AG$6+AG7)*AI$1+$AK$4)+$AK$4</f>
+        <f t="shared" ref="AH7:AH17" si="10">IF(AG7&lt;$AK$4/(AF$1),AG7*AF$1,(AG$6+AG7)*AI$1+$AK$4)+$AK$4</f>
         <v>1.4175757575757577</v>
       </c>
       <c r="AI7" s="41">
@@ -17687,18 +18918,18 @@
         <v>2</v>
       </c>
       <c r="C8" s="38">
-        <f t="shared" ref="C8:C17" si="9">C$6*2^B8</f>
+        <f t="shared" ref="C8:C17" si="11">C$6*2^B8</f>
         <v>0.156</v>
       </c>
       <c r="D8" s="36">
         <v>0.17100000000000001</v>
       </c>
       <c r="E8" s="42">
+        <f t="shared" si="1"/>
+        <v>5.9090909090909097E-2</v>
+      </c>
+      <c r="F8" s="42">
         <f t="shared" si="0"/>
-        <v>5.9090909090909097E-2</v>
-      </c>
-      <c r="F8" s="42">
-        <f>IF(E8&lt;($AK$4/(D$1)),(E$6+E8)*D$1,(E$6+E8)*G$1+$AK$4)+$AK$4</f>
         <v>1.5072727272727273</v>
       </c>
       <c r="G8" s="32">
@@ -17709,18 +18940,18 @@
         <v>2</v>
       </c>
       <c r="J8" s="38">
-        <f t="shared" ref="J8:J17" si="10">J$6*2^I8</f>
+        <f t="shared" ref="J8:J17" si="12">J$6*2^I8</f>
         <v>0.184</v>
       </c>
       <c r="K8" s="36">
         <v>0.191</v>
       </c>
       <c r="L8" s="42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.9696969696969702E-2</v>
       </c>
       <c r="M8" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
       <c r="N8" s="32">
@@ -17731,40 +18962,41 @@
         <v>2</v>
       </c>
       <c r="Q8" s="38">
-        <f t="shared" ref="Q8:Q17" si="11">Q$6*2^P8</f>
-        <v>0.15279999999999999</v>
+        <f t="shared" ref="Q8:Q17" si="13">Q$6*2^P8</f>
+        <v>0.2092</v>
       </c>
       <c r="R8" s="36">
-        <v>0.17</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="S8" s="42">
-        <f t="shared" si="3"/>
-        <v>5.7878787878787884E-2</v>
+        <f t="shared" si="4"/>
+        <v>7.9242424242424253E-2</v>
       </c>
       <c r="T8" s="42">
-        <f t="shared" si="4"/>
-        <v>1.2587878787878788</v>
-      </c>
-      <c r="U8" s="32">
-        <v>1.131</v>
+        <f t="shared" si="5"/>
+        <v>1.4392424242424244</v>
+      </c>
+      <c r="U8" s="38">
+        <f t="shared" si="6"/>
+        <v>0.15813427325858678</v>
       </c>
       <c r="V8" s="37"/>
       <c r="W8" s="33">
         <v>2</v>
       </c>
       <c r="X8" s="38">
-        <f t="shared" ref="X8:X17" si="12">X$6*2^W8</f>
+        <f t="shared" ref="X8:X17" si="14">X$6*2^W8</f>
         <v>0.152</v>
       </c>
       <c r="Y8" s="36">
         <v>0.16800000000000001</v>
       </c>
       <c r="Z8" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.7575757575757579E-2</v>
       </c>
       <c r="AA8" s="42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.87000000000000011</v>
       </c>
       <c r="AB8" s="33">
@@ -17775,18 +19007,18 @@
         <v>2</v>
       </c>
       <c r="AE8" s="38">
-        <f t="shared" ref="AE8:AE17" si="13">AE$6*2^AD8</f>
+        <f t="shared" ref="AE8:AE17" si="15">AE$6*2^AD8</f>
         <v>0.152</v>
       </c>
       <c r="AF8" s="36">
         <v>0.17100000000000001</v>
       </c>
       <c r="AG8" s="42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5.7575757575757579E-2</v>
       </c>
       <c r="AH8" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.4406060606060607</v>
       </c>
       <c r="AI8" s="41">
@@ -17799,18 +19031,18 @@
         <v>3</v>
       </c>
       <c r="C9" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.312</v>
       </c>
       <c r="D9" s="36">
         <v>0.34799999999999998</v>
       </c>
       <c r="E9" s="42">
+        <f t="shared" si="1"/>
+        <v>0.10636363636363637</v>
+      </c>
+      <c r="F9" s="42">
         <f t="shared" si="0"/>
-        <v>0.10636363636363637</v>
-      </c>
-      <c r="F9" s="42">
-        <f>IF(E9&lt;($AK$4/(D$1)),(E$6+E9)*D$1,(E$6+E9)*G$1+$AK$4)+$AK$4</f>
         <v>1.3600013</v>
       </c>
       <c r="G9" s="32">
@@ -17821,18 +19053,18 @@
         <v>3</v>
       </c>
       <c r="J9" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.36799999999999999</v>
       </c>
       <c r="K9" s="36">
         <v>0.39300000000000002</v>
       </c>
       <c r="L9" s="42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12545454545454546</v>
       </c>
       <c r="M9" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0940000000000001</v>
       </c>
       <c r="N9" s="32">
@@ -17843,40 +19075,41 @@
         <v>3</v>
       </c>
       <c r="Q9" s="38">
-        <f t="shared" si="11"/>
-        <v>0.30559999999999998</v>
+        <f t="shared" si="13"/>
+        <v>0.41839999999999999</v>
       </c>
       <c r="R9" s="36">
-        <v>0.35399999999999998</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="S9" s="42">
-        <f t="shared" si="3"/>
-        <v>0.10418181818181818</v>
+        <f t="shared" si="4"/>
+        <v>0.14263636363636364</v>
       </c>
       <c r="T9" s="42">
-        <f t="shared" si="4"/>
-        <v>1.4641818181818183</v>
-      </c>
-      <c r="U9" s="32">
-        <v>1.2529999999999999</v>
+        <f t="shared" si="5"/>
+        <v>1.5026363636363638</v>
+      </c>
+      <c r="U9" s="38">
+        <f t="shared" si="6"/>
+        <v>0.31600315420026737</v>
       </c>
       <c r="V9" s="37"/>
       <c r="W9" s="33">
         <v>3</v>
       </c>
       <c r="X9" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.30399999999999999</v>
       </c>
       <c r="Y9" s="36">
         <v>0.34799999999999998</v>
       </c>
       <c r="Z9" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.10363636363636364</v>
       </c>
       <c r="AA9" s="42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.022</v>
       </c>
       <c r="AB9" s="33">
@@ -17887,18 +19120,18 @@
         <v>3</v>
       </c>
       <c r="AE9" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.30399999999999999</v>
       </c>
       <c r="AF9" s="36">
         <v>0.35799999999999998</v>
       </c>
       <c r="AG9" s="42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.10363636363636364</v>
       </c>
       <c r="AH9" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.4866666666666668</v>
       </c>
       <c r="AI9" s="41">
@@ -17911,21 +19144,21 @@
         <v>4</v>
       </c>
       <c r="C10" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.624</v>
       </c>
       <c r="D10" s="36">
         <v>0.70899999999999996</v>
       </c>
       <c r="E10" s="42">
+        <f t="shared" si="1"/>
+        <v>0.20090909090909093</v>
+      </c>
+      <c r="F10" s="42">
         <f t="shared" si="0"/>
-        <v>0.20090909090909093</v>
-      </c>
-      <c r="F10" s="42">
-        <f>IF(E10&lt;($AK$4/(D$1)),(E$6+E10)*D$1,(E$6+E10)*G$1+$AK$4)+$AK$4</f>
         <v>1.3600022454545455</v>
       </c>
-      <c r="G10" s="47">
+      <c r="G10" s="45">
         <v>1.232</v>
       </c>
       <c r="H10" s="6"/>
@@ -17933,18 +19166,18 @@
         <v>4</v>
       </c>
       <c r="J10" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.73599999999999999</v>
       </c>
       <c r="K10" s="36">
         <v>0.82199999999999995</v>
       </c>
       <c r="L10" s="42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.236969696969697</v>
       </c>
       <c r="M10" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3600023696969696</v>
       </c>
       <c r="N10" s="32">
@@ -17955,40 +19188,41 @@
         <v>4</v>
       </c>
       <c r="Q10" s="38">
-        <f t="shared" si="11"/>
-        <v>0.61119999999999997</v>
+        <f t="shared" si="13"/>
+        <v>0.83679999999999999</v>
       </c>
       <c r="R10" s="36">
-        <v>0.71699999999999997</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="S10" s="42">
-        <f t="shared" si="3"/>
-        <v>0.19678787878787879</v>
+        <f t="shared" si="4"/>
+        <v>0.26942424242424245</v>
       </c>
       <c r="T10" s="42">
-        <f t="shared" si="4"/>
-        <v>1.5567878787878788</v>
-      </c>
-      <c r="U10" s="32">
-        <v>1.4139999999999999</v>
+        <f t="shared" si="5"/>
+        <v>1.6294242424242427</v>
+      </c>
+      <c r="U10" s="38">
+        <f t="shared" si="6"/>
+        <v>0.63147596916720683</v>
       </c>
       <c r="V10" s="37"/>
       <c r="W10" s="33">
         <v>4</v>
       </c>
       <c r="X10" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.60799999999999998</v>
       </c>
       <c r="Y10" s="36">
         <v>0.71299999999999997</v>
       </c>
       <c r="Z10" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.19575757575757577</v>
       </c>
       <c r="AA10" s="42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.3260000000000001</v>
       </c>
       <c r="AB10" s="33">
@@ -17999,18 +19233,18 @@
         <v>4</v>
       </c>
       <c r="AE10" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.60799999999999998</v>
       </c>
       <c r="AF10" s="36">
         <v>0.72699999999999998</v>
       </c>
       <c r="AG10" s="42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.19575757575757577</v>
       </c>
       <c r="AH10" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.5787878787878791</v>
       </c>
       <c r="AI10" s="41">
@@ -18023,18 +19257,18 @@
         <v>5</v>
       </c>
       <c r="C11" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.248</v>
       </c>
       <c r="D11" s="36">
         <v>1.44</v>
       </c>
       <c r="E11" s="42">
+        <f t="shared" si="1"/>
+        <v>0.39</v>
+      </c>
+      <c r="F11" s="42">
         <f t="shared" si="0"/>
-        <v>0.39</v>
-      </c>
-      <c r="F11" s="42">
-        <f>IF(E11&lt;($AK$4/(D$1)),(E$6+E11)*D$1,(E$6+E11)*G$1+$AK$4)+$AK$4</f>
         <v>1.3600041363636364</v>
       </c>
       <c r="G11" s="32">
@@ -18045,18 +19279,18 @@
         <v>5</v>
       </c>
       <c r="J11" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.472</v>
       </c>
       <c r="K11" s="36">
         <v>1.78</v>
       </c>
       <c r="L11" s="42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.46</v>
       </c>
       <c r="M11" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3600046000000001</v>
       </c>
       <c r="N11" s="32">
@@ -18067,40 +19301,41 @@
         <v>5</v>
       </c>
       <c r="Q11" s="38">
-        <f t="shared" si="11"/>
-        <v>1.2223999999999999</v>
+        <f t="shared" si="13"/>
+        <v>1.6736</v>
       </c>
       <c r="R11" s="36">
-        <v>1.4550000000000001</v>
+        <v>1.6779999999999999</v>
       </c>
       <c r="S11" s="42">
-        <f t="shared" si="3"/>
-        <v>0.38200000000000001</v>
+        <f t="shared" si="4"/>
+        <v>0.52300000000000002</v>
       </c>
       <c r="T11" s="42">
-        <f t="shared" si="4"/>
-        <v>1.742</v>
-      </c>
-      <c r="U11" s="32">
-        <v>1.7050000000000001</v>
+        <f t="shared" si="5"/>
+        <v>1.883</v>
+      </c>
+      <c r="U11" s="38">
+        <f t="shared" si="6"/>
+        <v>1.2618921499212232</v>
       </c>
       <c r="V11" s="37"/>
       <c r="W11" s="33">
         <v>5</v>
       </c>
       <c r="X11" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.216</v>
       </c>
       <c r="Y11" s="36">
         <v>1.4670000000000001</v>
       </c>
       <c r="Z11" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.38</v>
       </c>
       <c r="AA11" s="42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.9340000000000002</v>
       </c>
       <c r="AB11" s="33">
@@ -18111,18 +19346,18 @@
         <v>5</v>
       </c>
       <c r="AE11" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.216</v>
       </c>
       <c r="AF11" s="36">
         <v>1.484</v>
       </c>
       <c r="AG11" s="42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.38</v>
       </c>
       <c r="AH11" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.7630303030303032</v>
       </c>
       <c r="AI11" s="41">
@@ -18135,18 +19370,18 @@
         <v>6</v>
       </c>
       <c r="C12" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2.496</v>
       </c>
       <c r="D12" s="36">
         <v>2.84</v>
       </c>
       <c r="E12" s="42">
+        <f t="shared" si="1"/>
+        <v>0.7681818181818183</v>
+      </c>
+      <c r="F12" s="42">
         <f t="shared" si="0"/>
-        <v>0.7681818181818183</v>
-      </c>
-      <c r="F12" s="42">
-        <f>IF(E12&lt;($AK$4/(D$1)),(E$6+E12)*D$1,(E$6+E12)*G$1+$AK$4)+$AK$4</f>
         <v>1.3600079181818183</v>
       </c>
       <c r="G12" s="32">
@@ -18157,18 +19392,18 @@
         <v>6</v>
       </c>
       <c r="J12" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.944</v>
       </c>
       <c r="K12" s="36">
         <v>3.65</v>
       </c>
       <c r="L12" s="42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.90606060606060601</v>
       </c>
       <c r="M12" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3600090606060609</v>
       </c>
       <c r="N12" s="32">
@@ -18179,40 +19414,41 @@
         <v>6</v>
       </c>
       <c r="Q12" s="38">
-        <f t="shared" si="11"/>
-        <v>2.4447999999999999</v>
+        <f t="shared" si="13"/>
+        <v>3.3472</v>
       </c>
       <c r="R12" s="36">
-        <v>2.89</v>
+        <v>3.37</v>
       </c>
       <c r="S12" s="42">
-        <f t="shared" si="3"/>
-        <v>0.75242424242424233</v>
+        <f t="shared" si="4"/>
+        <v>1.030151515151515</v>
       </c>
       <c r="T12" s="42">
-        <f t="shared" si="4"/>
-        <v>2.1124242424242423</v>
-      </c>
-      <c r="U12" s="32">
-        <v>2.21</v>
+        <f t="shared" si="5"/>
+        <v>2.3901515151515151</v>
+      </c>
+      <c r="U12" s="38">
+        <f t="shared" si="6"/>
+        <v>2.5216665016292414</v>
       </c>
       <c r="V12" s="37"/>
       <c r="W12" s="33">
         <v>6</v>
       </c>
       <c r="X12" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2.4319999999999999</v>
       </c>
       <c r="Y12" s="36">
         <v>2.89</v>
       </c>
       <c r="Z12" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.74848484848484842</v>
       </c>
       <c r="AA12" s="42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.15</v>
       </c>
       <c r="AB12" s="33">
@@ -18223,18 +19459,18 @@
         <v>6</v>
       </c>
       <c r="AE12" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2.4319999999999999</v>
       </c>
       <c r="AF12" s="36">
         <v>2.94</v>
       </c>
       <c r="AG12" s="42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.74848484848484842</v>
       </c>
       <c r="AH12" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.1315151515151518</v>
       </c>
       <c r="AI12" s="41">
@@ -18247,18 +19483,18 @@
         <v>7</v>
       </c>
       <c r="C13" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4.992</v>
       </c>
       <c r="D13" s="36">
         <v>5.5</v>
       </c>
       <c r="E13" s="42">
+        <f t="shared" si="1"/>
+        <v>1.5245454545454544</v>
+      </c>
+      <c r="F13" s="42">
         <f t="shared" si="0"/>
-        <v>1.5245454545454544</v>
-      </c>
-      <c r="F13" s="42">
-        <f>IF(E13&lt;($AK$4/(D$1)),(E$6+E13)*D$1,(E$6+E13)*G$1+$AK$4)+$AK$4</f>
         <v>1.360015481818182</v>
       </c>
       <c r="G13" s="32">
@@ -18269,18 +19505,18 @@
         <v>7</v>
       </c>
       <c r="J13" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5.8879999999999999</v>
       </c>
       <c r="K13" s="36">
         <v>6.26</v>
       </c>
       <c r="L13" s="42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7981818181818183</v>
       </c>
       <c r="M13" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3600179818181819</v>
       </c>
       <c r="N13" s="32">
@@ -18291,40 +19527,41 @@
         <v>7</v>
       </c>
       <c r="Q13" s="38">
-        <f t="shared" si="11"/>
-        <v>4.8895999999999997</v>
+        <f t="shared" si="13"/>
+        <v>6.6943999999999999</v>
       </c>
       <c r="R13" s="36">
-        <v>5.48</v>
+        <v>6.81</v>
       </c>
       <c r="S13" s="42">
-        <f t="shared" si="3"/>
-        <v>1.4932727272727273</v>
+        <f t="shared" si="4"/>
+        <v>2.0444545454545455</v>
       </c>
       <c r="T13" s="42">
-        <f t="shared" si="4"/>
-        <v>2.8532727272727274</v>
-      </c>
-      <c r="U13" s="32">
-        <v>3.12</v>
+        <f t="shared" si="5"/>
+        <v>3.4044545454545458</v>
+      </c>
+      <c r="U13" s="38">
+        <f t="shared" si="6"/>
+        <v>5.0391009610734425</v>
       </c>
       <c r="V13" s="37"/>
       <c r="W13" s="33">
         <v>7</v>
       </c>
       <c r="X13" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>4.8639999999999999</v>
       </c>
       <c r="Y13" s="36">
         <v>5.59</v>
       </c>
       <c r="Z13" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.4854545454545456</v>
       </c>
       <c r="AA13" s="42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5.5819999999999999</v>
       </c>
       <c r="AB13" s="33">
@@ -18335,18 +19572,18 @@
         <v>7</v>
       </c>
       <c r="AE13" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4.8639999999999999</v>
       </c>
       <c r="AF13" s="36">
         <v>5.68</v>
       </c>
       <c r="AG13" s="42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.4854545454545456</v>
       </c>
       <c r="AH13" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.8684848484848486</v>
       </c>
       <c r="AI13" s="41">
@@ -18359,18 +19596,18 @@
         <v>8</v>
       </c>
       <c r="C14" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>9.984</v>
       </c>
       <c r="D14" s="36">
         <v>10.14</v>
       </c>
       <c r="E14" s="42">
+        <f t="shared" si="1"/>
+        <v>3.0372727272727271</v>
+      </c>
+      <c r="F14" s="42">
         <f t="shared" si="0"/>
-        <v>3.0372727272727271</v>
-      </c>
-      <c r="F14" s="42">
-        <f>IF(E14&lt;($AK$4/(D$1)),(E$6+E14)*D$1,(E$6+E14)*G$1+$AK$4)+$AK$4</f>
         <v>1.3600306090909093</v>
       </c>
       <c r="G14" s="32">
@@ -18381,18 +19618,18 @@
         <v>7.75</v>
       </c>
       <c r="J14" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>9.9023961860277439</v>
       </c>
       <c r="K14" s="36">
         <v>10.45</v>
       </c>
       <c r="L14" s="42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.014665510917498</v>
       </c>
       <c r="M14" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3600301466551092</v>
       </c>
       <c r="N14" s="32">
@@ -18400,43 +19637,44 @@
       </c>
       <c r="O14" s="37"/>
       <c r="P14" s="32">
-        <v>8</v>
+        <v>7.64</v>
       </c>
       <c r="Q14" s="38">
-        <f t="shared" si="11"/>
-        <v>9.7791999999999994</v>
-      </c>
-      <c r="R14" s="36">
-        <v>10.24</v>
+        <f t="shared" si="13"/>
+        <v>10.432078724158499</v>
+      </c>
+      <c r="R14" s="46">
+        <v>10.45</v>
       </c>
       <c r="S14" s="42">
-        <f t="shared" si="3"/>
-        <v>2.9749696969696968</v>
+        <f t="shared" si="4"/>
+        <v>3.1770844618662122</v>
       </c>
       <c r="T14" s="42">
-        <f t="shared" si="4"/>
-        <v>4.3349696969696971</v>
-      </c>
-      <c r="U14" s="32">
-        <v>4.63</v>
+        <f t="shared" si="5"/>
+        <v>4.5370844618662121</v>
+      </c>
+      <c r="U14" s="38">
+        <f t="shared" si="6"/>
+        <v>7.8483601235209406</v>
       </c>
       <c r="V14" s="37"/>
       <c r="W14" s="33">
         <v>8</v>
       </c>
       <c r="X14" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>9.7279999999999998</v>
       </c>
       <c r="Y14" s="36">
         <v>10.09</v>
       </c>
       <c r="Z14" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.9593939393939395</v>
       </c>
       <c r="AA14" s="42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>10.446</v>
       </c>
       <c r="AB14" s="33">
@@ -18447,18 +19685,18 @@
         <v>8</v>
       </c>
       <c r="AE14" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>9.7279999999999998</v>
       </c>
       <c r="AF14" s="36">
         <v>10.37</v>
       </c>
       <c r="AG14" s="42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.9593939393939395</v>
       </c>
       <c r="AH14" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.3424242424242427</v>
       </c>
       <c r="AI14" s="41">
@@ -18471,18 +19709,18 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="C15" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>10.336084999632316</v>
       </c>
       <c r="D15" s="36">
         <v>10.45</v>
       </c>
       <c r="E15" s="42">
+        <f t="shared" si="1"/>
+        <v>3.1439651514037323</v>
+      </c>
+      <c r="F15" s="42">
         <f t="shared" si="0"/>
-        <v>3.1439651514037323</v>
-      </c>
-      <c r="F15" s="42">
-        <f>IF(E15&lt;($AK$4/(D$1)),(E$6+E15)*D$1,(E$6+E15)*G$1+$AK$4)+$AK$4</f>
         <v>1.3600316760151505</v>
       </c>
       <c r="G15" s="41">
@@ -18493,18 +19731,18 @@
         <v>8</v>
       </c>
       <c r="J15" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>11.776</v>
       </c>
       <c r="K15" s="36">
         <v>10.45</v>
       </c>
       <c r="L15" s="42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.5824242424242425</v>
       </c>
       <c r="M15" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3600358242424244</v>
       </c>
       <c r="N15" s="32">
@@ -18512,43 +19750,44 @@
       </c>
       <c r="O15" s="37"/>
       <c r="P15" s="32">
-        <v>8.0399999999999991</v>
+        <v>8</v>
       </c>
       <c r="Q15" s="38">
-        <f t="shared" si="11"/>
-        <v>10.054130733634997</v>
-      </c>
-      <c r="R15" s="36">
-        <v>10.33</v>
+        <f t="shared" si="13"/>
+        <v>13.3888</v>
+      </c>
+      <c r="R15" s="46">
+        <v>10.45</v>
       </c>
       <c r="S15" s="42">
-        <f t="shared" si="3"/>
-        <v>3.0582820404954538</v>
+        <f t="shared" si="4"/>
+        <v>4.073060606060606</v>
       </c>
       <c r="T15" s="42">
-        <f t="shared" si="4"/>
-        <v>4.4182820404954537</v>
-      </c>
-      <c r="U15" s="32">
-        <v>4.68</v>
+        <f t="shared" si="5"/>
+        <v>5.4330606060606055</v>
+      </c>
+      <c r="U15" s="38">
+        <f t="shared" si="6"/>
+        <v>10.069744940294523</v>
       </c>
       <c r="V15" s="37"/>
       <c r="W15" s="33">
         <v>8.0399999999999991</v>
       </c>
       <c r="X15" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>10.001491305710207</v>
       </c>
       <c r="Y15" s="36">
         <v>10.25</v>
       </c>
       <c r="Z15" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.0422700926394568</v>
       </c>
       <c r="AA15" s="42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>10.719491305710207</v>
       </c>
       <c r="AB15" s="41">
@@ -18559,18 +19798,18 @@
         <v>8.0399999999999991</v>
       </c>
       <c r="AE15" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.001491305710207</v>
       </c>
       <c r="AF15" s="36">
         <v>10.45</v>
       </c>
       <c r="AG15" s="42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.0422700926394568</v>
       </c>
       <c r="AH15" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.4253003956697601</v>
       </c>
       <c r="AI15" s="41">
@@ -18583,18 +19822,18 @@
         <v>9</v>
       </c>
       <c r="C16" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>19.968</v>
       </c>
       <c r="D16" s="36">
         <v>10.45</v>
       </c>
       <c r="E16" s="42">
+        <f t="shared" si="1"/>
+        <v>6.0627272727272734</v>
+      </c>
+      <c r="F16" s="42">
         <f t="shared" si="0"/>
-        <v>6.0627272727272734</v>
-      </c>
-      <c r="F16" s="42">
-        <f>IF(E16&lt;($AK$4/(D$1)),(E$6+E16)*D$1,(E$6+E16)*G$1+$AK$4)+$AK$4</f>
         <v>1.3600608636363636</v>
       </c>
       <c r="G16" s="32">
@@ -18605,18 +19844,18 @@
         <v>9</v>
       </c>
       <c r="J16" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>23.552</v>
       </c>
       <c r="K16" s="36">
         <v>10.45</v>
       </c>
       <c r="L16" s="42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.1509090909090913</v>
       </c>
       <c r="M16" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3600715090909092</v>
       </c>
       <c r="N16" s="32">
@@ -18627,40 +19866,41 @@
         <v>9</v>
       </c>
       <c r="Q16" s="38">
-        <f t="shared" si="11"/>
-        <v>19.558399999999999</v>
-      </c>
-      <c r="R16" s="36">
-        <v>10.38</v>
+        <f t="shared" si="13"/>
+        <v>26.7776</v>
+      </c>
+      <c r="R16" s="46">
+        <v>10.45</v>
       </c>
       <c r="S16" s="42">
-        <f t="shared" si="3"/>
-        <v>5.9383636363636363</v>
+        <f t="shared" si="4"/>
+        <v>8.1302727272727271</v>
       </c>
       <c r="T16" s="42">
-        <f t="shared" si="4"/>
-        <v>7.2983636363636357</v>
-      </c>
-      <c r="U16" s="32">
-        <v>5.62</v>
+        <f t="shared" si="5"/>
+        <v>9.4902727272727265</v>
+      </c>
+      <c r="U16" s="38">
+        <f t="shared" si="6"/>
+        <v>20.122590109999848</v>
       </c>
       <c r="V16" s="37"/>
       <c r="W16" s="33">
         <v>9</v>
       </c>
       <c r="X16" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>19.456</v>
       </c>
       <c r="Y16" s="36">
         <v>10.25</v>
       </c>
       <c r="Z16" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.9072727272727272</v>
       </c>
       <c r="AA16" s="42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20.173999999999999</v>
       </c>
       <c r="AB16" s="33">
@@ -18671,18 +19911,18 @@
         <v>9</v>
       </c>
       <c r="AE16" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>19.456</v>
       </c>
       <c r="AF16" s="36">
         <v>10.45</v>
       </c>
       <c r="AG16" s="42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5.9072727272727272</v>
       </c>
       <c r="AH16" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>7.2903030303030301</v>
       </c>
       <c r="AI16" s="41">
@@ -18695,18 +19935,18 @@
         <v>10</v>
       </c>
       <c r="C17" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>39.936</v>
       </c>
       <c r="D17" s="36">
         <v>10.45</v>
       </c>
       <c r="E17" s="42">
+        <f t="shared" si="1"/>
+        <v>12.113636363636365</v>
+      </c>
+      <c r="F17" s="42">
         <f t="shared" si="0"/>
-        <v>12.113636363636365</v>
-      </c>
-      <c r="F17" s="42">
-        <f>IF(E17&lt;($AK$4/(D$1)),(E$6+E17)*D$1,(E$6+E17)*G$1+$AK$4)+$AK$4</f>
         <v>1.360121372727273</v>
       </c>
       <c r="G17" s="32">
@@ -18717,18 +19957,18 @@
         <v>10</v>
       </c>
       <c r="J17" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>47.103999999999999</v>
       </c>
       <c r="K17" s="36">
         <v>10.45</v>
       </c>
       <c r="L17" s="42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.287878787878789</v>
       </c>
       <c r="M17" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3601428787878789</v>
       </c>
       <c r="N17" s="32">
@@ -18739,40 +19979,41 @@
         <v>10</v>
       </c>
       <c r="Q17" s="38">
-        <f t="shared" si="11"/>
-        <v>39.116799999999998</v>
-      </c>
-      <c r="R17" s="36">
-        <v>10.39</v>
+        <f t="shared" si="13"/>
+        <v>53.555199999999999</v>
+      </c>
+      <c r="R17" s="46">
+        <v>10.45</v>
       </c>
       <c r="S17" s="42">
-        <f t="shared" si="3"/>
-        <v>11.865151515151517</v>
+        <f t="shared" si="4"/>
+        <v>16.244696969696971</v>
       </c>
       <c r="T17" s="42">
-        <f t="shared" si="4"/>
-        <v>13.225151515151516</v>
-      </c>
-      <c r="U17" s="32">
-        <v>6.74</v>
+        <f t="shared" si="5"/>
+        <v>17.60469696969697</v>
+      </c>
+      <c r="U17" s="38">
+        <f t="shared" si="6"/>
+        <v>40.211409041232486</v>
       </c>
       <c r="V17" s="37"/>
       <c r="W17" s="33">
         <v>10</v>
       </c>
       <c r="X17" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>38.911999999999999</v>
       </c>
       <c r="Y17" s="36">
         <v>10.25</v>
       </c>
       <c r="Z17" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>11.803030303030303</v>
       </c>
       <c r="AA17" s="42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>39.629999999999995</v>
       </c>
       <c r="AB17" s="33">
@@ -18783,18 +20024,18 @@
         <v>10</v>
       </c>
       <c r="AE17" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>38.911999999999999</v>
       </c>
       <c r="AF17" s="36">
         <v>10.45</v>
       </c>
       <c r="AG17" s="42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>11.803030303030303</v>
       </c>
       <c r="AH17" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>13.186060606060606</v>
       </c>
       <c r="AI17" s="41">
@@ -18851,11 +20092,11 @@
       </c>
       <c r="S49" s="42">
         <f>(Q$6+Q49)/3.3</f>
-        <v>2.4909090909090909E-2</v>
+        <v>2.9181818181818184E-2</v>
       </c>
       <c r="T49" s="42">
-        <f>IF(S49&lt;$AK$4/(R$1),(S$6+S49)*R$1,(S$6+S49)*U$1+$AK$4)+$AK$4</f>
-        <v>1.1606060606060606</v>
+        <f t="shared" ref="T49:T60" si="16">IF(S49&lt;$AK$4/(R$1),(S$6+S49)*R$1,(S$6+S49)*U$1+$AK$4)+$AK$4</f>
+        <v>1.2887878787878788</v>
       </c>
       <c r="U49" s="41">
         <v>0.79</v>
@@ -18867,18 +20108,18 @@
       </c>
       <c r="Q50" s="38">
         <f>Q$6*2^P50</f>
-        <v>7.6399999999999996E-2</v>
+        <v>0.1046</v>
       </c>
       <c r="R50" s="36">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="S50" s="42">
-        <f t="shared" ref="S50:S60" si="14">(Q$6+Q50)/3.3</f>
-        <v>3.4727272727272725E-2</v>
+        <f t="shared" ref="S50:S60" si="17">(Q$6+Q50)/3.3</f>
+        <v>4.7545454545454544E-2</v>
       </c>
       <c r="T50" s="42">
-        <f>IF(S50&lt;$AK$4/(R$1),(S$6+S50)*R$1,(S$6+S50)*U$1+$AK$4)+$AK$4</f>
-        <v>1.2587878787878788</v>
+        <f t="shared" si="16"/>
+        <v>1.4724242424242424</v>
       </c>
       <c r="U50" s="41">
         <v>0.94</v>
@@ -18889,19 +20130,19 @@
         <v>2</v>
       </c>
       <c r="Q51" s="38">
-        <f t="shared" ref="Q51:Q60" si="15">Q$6*2^P51</f>
-        <v>0.15279999999999999</v>
+        <f t="shared" ref="Q51:Q60" si="18">Q$6*2^P51</f>
+        <v>0.2092</v>
       </c>
       <c r="R51" s="36">
         <v>0.17</v>
       </c>
       <c r="S51" s="42">
-        <f t="shared" si="14"/>
-        <v>5.7878787878787884E-2</v>
+        <f t="shared" si="17"/>
+        <v>7.9242424242424253E-2</v>
       </c>
       <c r="T51" s="42">
-        <f>IF(S51&lt;$AK$4/(R$1),(S$6+S51)*R$1,(S$6+S51)*U$1+$AK$4)+$AK$4</f>
-        <v>1.4903030303030302</v>
+        <f t="shared" si="16"/>
+        <v>1.470939393939394</v>
       </c>
       <c r="U51" s="41">
         <v>1.1299999999999999</v>
@@ -18912,19 +20153,19 @@
         <v>3</v>
       </c>
       <c r="Q52" s="38">
-        <f t="shared" si="15"/>
-        <v>0.30559999999999998</v>
+        <f t="shared" si="18"/>
+        <v>0.41839999999999999</v>
       </c>
       <c r="R52" s="36">
         <v>0.35299999999999998</v>
       </c>
       <c r="S52" s="42">
-        <f t="shared" si="14"/>
-        <v>0.10418181818181818</v>
+        <f t="shared" si="17"/>
+        <v>0.14263636363636364</v>
       </c>
       <c r="T52" s="42">
-        <f>IF(S52&lt;$AK$4/(R$1),(S$6+S52)*R$1,(S$6+S52)*U$1+$AK$4)+$AK$4</f>
-        <v>1.4873333333333334</v>
+        <f t="shared" si="16"/>
+        <v>1.5343333333333335</v>
       </c>
       <c r="U52" s="41">
         <v>1.23</v>
@@ -18935,19 +20176,19 @@
         <v>4</v>
       </c>
       <c r="Q53" s="38">
-        <f t="shared" si="15"/>
-        <v>0.61119999999999997</v>
+        <f t="shared" si="18"/>
+        <v>0.83679999999999999</v>
       </c>
       <c r="R53" s="36">
         <v>0.72499999999999998</v>
       </c>
       <c r="S53" s="42">
-        <f t="shared" si="14"/>
-        <v>0.19678787878787879</v>
+        <f t="shared" si="17"/>
+        <v>0.26942424242424245</v>
       </c>
       <c r="T53" s="42">
-        <f>IF(S53&lt;$AK$4/(R$1),(S$6+S53)*R$1,(S$6+S53)*U$1+$AK$4)+$AK$4</f>
-        <v>1.579939393939394</v>
+        <f t="shared" si="16"/>
+        <v>1.6611212121212122</v>
       </c>
       <c r="U53" s="41">
         <v>1.45</v>
@@ -18958,19 +20199,19 @@
         <v>5</v>
       </c>
       <c r="Q54" s="38">
-        <f t="shared" si="15"/>
-        <v>1.2223999999999999</v>
+        <f t="shared" si="18"/>
+        <v>1.6736</v>
       </c>
       <c r="R54" s="36">
         <v>1.448</v>
       </c>
       <c r="S54" s="42">
-        <f t="shared" si="14"/>
-        <v>0.38200000000000001</v>
+        <f t="shared" si="17"/>
+        <v>0.52300000000000002</v>
       </c>
       <c r="T54" s="42">
-        <f>IF(S54&lt;$AK$4/(R$1),(S$6+S54)*R$1,(S$6+S54)*U$1+$AK$4)+$AK$4</f>
-        <v>1.7651515151515151</v>
+        <f t="shared" si="16"/>
+        <v>1.91469696969697</v>
       </c>
       <c r="U54" s="41">
         <v>1.76</v>
@@ -18981,19 +20222,19 @@
         <v>6</v>
       </c>
       <c r="Q55" s="38">
-        <f t="shared" si="15"/>
-        <v>2.4447999999999999</v>
+        <f t="shared" si="18"/>
+        <v>3.3472</v>
       </c>
       <c r="R55" s="36">
         <v>2.87</v>
       </c>
       <c r="S55" s="42">
-        <f t="shared" si="14"/>
-        <v>0.75242424242424233</v>
+        <f t="shared" si="17"/>
+        <v>1.030151515151515</v>
       </c>
       <c r="T55" s="42">
-        <f>IF(S55&lt;$AK$4/(R$1),(S$6+S55)*R$1,(S$6+S55)*U$1+$AK$4)+$AK$4</f>
-        <v>2.1355757575757575</v>
+        <f t="shared" si="16"/>
+        <v>2.4218484848484851</v>
       </c>
       <c r="U55" s="41">
         <v>2.2999999999999998</v>
@@ -19004,19 +20245,19 @@
         <v>7</v>
       </c>
       <c r="Q56" s="38">
-        <f t="shared" si="15"/>
-        <v>4.8895999999999997</v>
+        <f t="shared" si="18"/>
+        <v>6.6943999999999999</v>
       </c>
       <c r="R56" s="36">
         <v>5.58</v>
       </c>
       <c r="S56" s="42">
-        <f t="shared" si="14"/>
-        <v>1.4932727272727273</v>
+        <f t="shared" si="17"/>
+        <v>2.0444545454545455</v>
       </c>
       <c r="T56" s="42">
-        <f>IF(S56&lt;$AK$4/(R$1),(S$6+S56)*R$1,(S$6+S56)*U$1+$AK$4)+$AK$4</f>
-        <v>2.8764242424242425</v>
+        <f t="shared" si="16"/>
+        <v>3.4361515151515154</v>
       </c>
       <c r="U56" s="41">
         <v>3.27</v>
@@ -19027,19 +20268,19 @@
         <v>8</v>
       </c>
       <c r="Q57" s="38">
-        <f t="shared" si="15"/>
-        <v>9.7791999999999994</v>
+        <f t="shared" si="18"/>
+        <v>13.3888</v>
       </c>
       <c r="R57" s="36">
         <v>10.29</v>
       </c>
       <c r="S57" s="42">
-        <f t="shared" si="14"/>
-        <v>2.9749696969696968</v>
+        <f t="shared" si="17"/>
+        <v>4.073060606060606</v>
       </c>
       <c r="T57" s="42">
-        <f>IF(S57&lt;$AK$4/(R$1),(S$6+S57)*R$1,(S$6+S57)*U$1+$AK$4)+$AK$4</f>
-        <v>4.3581212121212118</v>
+        <f t="shared" si="16"/>
+        <v>5.4647575757575755</v>
       </c>
       <c r="U57" s="41">
         <v>4.8</v>
@@ -19050,19 +20291,19 @@
         <v>8.0399999999999991</v>
       </c>
       <c r="Q58" s="38">
-        <f t="shared" si="15"/>
-        <v>10.054130733634997</v>
+        <f t="shared" si="18"/>
+        <v>13.765210402332732</v>
       </c>
       <c r="R58" s="36">
         <v>10.45</v>
       </c>
       <c r="S58" s="42">
-        <f t="shared" si="14"/>
-        <v>3.0582820404954538</v>
+        <f t="shared" si="17"/>
+        <v>4.1871243643432523</v>
       </c>
       <c r="T58" s="42">
-        <f>IF(S58&lt;$AK$4/(R$1),(S$6+S58)*R$1,(S$6+S58)*U$1+$AK$4)+$AK$4</f>
-        <v>4.4414335556469693</v>
+        <f t="shared" si="16"/>
+        <v>5.5788213340402217</v>
       </c>
       <c r="U58" s="41">
         <v>4.91</v>
@@ -19073,19 +20314,19 @@
         <v>9</v>
       </c>
       <c r="Q59" s="38">
-        <f t="shared" si="15"/>
-        <v>19.558399999999999</v>
+        <f t="shared" si="18"/>
+        <v>26.7776</v>
       </c>
       <c r="R59" s="36">
         <v>10.45</v>
       </c>
       <c r="S59" s="42">
-        <f t="shared" si="14"/>
-        <v>5.9383636363636363</v>
+        <f t="shared" si="17"/>
+        <v>8.1302727272727271</v>
       </c>
       <c r="T59" s="42">
-        <f>IF(S59&lt;$AK$4/(R$1),(S$6+S59)*R$1,(S$6+S59)*U$1+$AK$4)+$AK$4</f>
-        <v>7.3215151515151513</v>
+        <f t="shared" si="16"/>
+        <v>9.5219696969696965</v>
       </c>
       <c r="U59" s="41">
         <v>5.8</v>
@@ -19096,22 +20337,336 @@
         <v>10</v>
       </c>
       <c r="Q60" s="38">
-        <f t="shared" si="15"/>
-        <v>39.116799999999998</v>
+        <f t="shared" si="18"/>
+        <v>53.555199999999999</v>
       </c>
       <c r="R60" s="36">
         <v>10.45</v>
       </c>
       <c r="S60" s="42">
-        <f t="shared" si="14"/>
-        <v>11.865151515151517</v>
+        <f t="shared" si="17"/>
+        <v>16.244696969696971</v>
       </c>
       <c r="T60" s="42">
-        <f>IF(S60&lt;$AK$4/(R$1),(S$6+S60)*R$1,(S$6+S60)*U$1+$AK$4)+$AK$4</f>
-        <v>13.248303030303031</v>
+        <f t="shared" si="16"/>
+        <v>17.63639393939394</v>
       </c>
       <c r="U60" s="41">
         <v>6.73</v>
+      </c>
+    </row>
+    <row r="62" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P62" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q62" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="R62" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="S62" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="T62" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="U62" s="43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P63" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q63" s="27"/>
+      <c r="R63" s="27"/>
+      <c r="S63" s="27"/>
+      <c r="T63" s="27"/>
+      <c r="U63" s="29"/>
+    </row>
+    <row r="64" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P64" s="6"/>
+      <c r="Q64" s="6"/>
+      <c r="R64" s="6"/>
+      <c r="S64" s="6"/>
+      <c r="T64" s="6"/>
+      <c r="U64" s="6"/>
+    </row>
+    <row r="65" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P65" s="43">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="43">
+        <f>R65</f>
+        <v>3.8199999999999998E-2</v>
+      </c>
+      <c r="R65" s="36">
+        <v>3.8199999999999998E-2</v>
+      </c>
+      <c r="S65" s="42">
+        <f>(Q$6+Q65)/3.3</f>
+        <v>2.7424242424242424E-2</v>
+      </c>
+      <c r="T65" s="42">
+        <f>IF(S65&lt;$AK$4/(R$1),S65*R$1,S65*U$1+$AK$4)+$AK$4</f>
+        <v>0.95424242424242434</v>
+      </c>
+      <c r="U65" s="43">
+        <v>0.78600000000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P66" s="43">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="38">
+        <f>Q$6*2^P66</f>
+        <v>0.1046</v>
+      </c>
+      <c r="R66" s="36">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="S66" s="42">
+        <f t="shared" ref="S66:S76" si="19">(Q$6+Q66)/3.3</f>
+        <v>4.7545454545454544E-2</v>
+      </c>
+      <c r="T66" s="42">
+        <f t="shared" ref="T66:T76" si="20">IF(S66&lt;$AK$4/(R$1),S66*R$1,S66*U$1+$AK$4)+$AK$4</f>
+        <v>1.1554545454545455</v>
+      </c>
+      <c r="U66" s="43">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="67" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P67" s="43">
+        <v>2</v>
+      </c>
+      <c r="Q67" s="38">
+        <f t="shared" ref="Q67:Q76" si="21">Q$6*2^P67</f>
+        <v>0.2092</v>
+      </c>
+      <c r="R67" s="36">
+        <v>0.17</v>
+      </c>
+      <c r="S67" s="42">
+        <f t="shared" si="19"/>
+        <v>7.9242424242424253E-2</v>
+      </c>
+      <c r="T67" s="42">
+        <f t="shared" si="20"/>
+        <v>1.4392424242424244</v>
+      </c>
+      <c r="U67" s="43">
+        <v>1.131</v>
+      </c>
+    </row>
+    <row r="68" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P68" s="43">
+        <v>3</v>
+      </c>
+      <c r="Q68" s="38">
+        <f t="shared" si="21"/>
+        <v>0.41839999999999999</v>
+      </c>
+      <c r="R68" s="36">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="S68" s="42">
+        <f t="shared" si="19"/>
+        <v>0.14263636363636364</v>
+      </c>
+      <c r="T68" s="42">
+        <f t="shared" si="20"/>
+        <v>1.5026363636363638</v>
+      </c>
+      <c r="U68" s="43">
+        <v>1.2529999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P69" s="43">
+        <v>4</v>
+      </c>
+      <c r="Q69" s="38">
+        <f t="shared" si="21"/>
+        <v>0.83679999999999999</v>
+      </c>
+      <c r="R69" s="36">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="S69" s="42">
+        <f t="shared" si="19"/>
+        <v>0.26942424242424245</v>
+      </c>
+      <c r="T69" s="42">
+        <f t="shared" si="20"/>
+        <v>1.6294242424242427</v>
+      </c>
+      <c r="U69" s="43">
+        <v>1.4139999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P70" s="43">
+        <v>5</v>
+      </c>
+      <c r="Q70" s="38">
+        <f t="shared" si="21"/>
+        <v>1.6736</v>
+      </c>
+      <c r="R70" s="36">
+        <v>1.4550000000000001</v>
+      </c>
+      <c r="S70" s="42">
+        <f t="shared" si="19"/>
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="T70" s="42">
+        <f t="shared" si="20"/>
+        <v>1.883</v>
+      </c>
+      <c r="U70" s="43">
+        <v>1.7050000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P71" s="43">
+        <v>6</v>
+      </c>
+      <c r="Q71" s="38">
+        <f t="shared" si="21"/>
+        <v>3.3472</v>
+      </c>
+      <c r="R71" s="36">
+        <v>2.89</v>
+      </c>
+      <c r="S71" s="42">
+        <f t="shared" si="19"/>
+        <v>1.030151515151515</v>
+      </c>
+      <c r="T71" s="42">
+        <f t="shared" si="20"/>
+        <v>2.3901515151515151</v>
+      </c>
+      <c r="U71" s="43">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="72" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P72" s="43">
+        <v>7</v>
+      </c>
+      <c r="Q72" s="38">
+        <f t="shared" si="21"/>
+        <v>6.6943999999999999</v>
+      </c>
+      <c r="R72" s="36">
+        <v>5.48</v>
+      </c>
+      <c r="S72" s="42">
+        <f t="shared" si="19"/>
+        <v>2.0444545454545455</v>
+      </c>
+      <c r="T72" s="42">
+        <f t="shared" si="20"/>
+        <v>3.4044545454545458</v>
+      </c>
+      <c r="U72" s="43">
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="73" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P73" s="43">
+        <v>8</v>
+      </c>
+      <c r="Q73" s="38">
+        <f t="shared" si="21"/>
+        <v>13.3888</v>
+      </c>
+      <c r="R73" s="36">
+        <v>10.24</v>
+      </c>
+      <c r="S73" s="42">
+        <f t="shared" si="19"/>
+        <v>4.073060606060606</v>
+      </c>
+      <c r="T73" s="42">
+        <f t="shared" si="20"/>
+        <v>5.4330606060606055</v>
+      </c>
+      <c r="U73" s="43">
+        <v>4.63</v>
+      </c>
+    </row>
+    <row r="74" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P74" s="43">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="Q74" s="38">
+        <f t="shared" si="21"/>
+        <v>13.765210402332732</v>
+      </c>
+      <c r="R74" s="36">
+        <v>10.33</v>
+      </c>
+      <c r="S74" s="42">
+        <f t="shared" si="19"/>
+        <v>4.1871243643432523</v>
+      </c>
+      <c r="T74" s="42">
+        <f t="shared" si="20"/>
+        <v>5.5471243643432517</v>
+      </c>
+      <c r="U74" s="43">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="75" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P75" s="43">
+        <v>9</v>
+      </c>
+      <c r="Q75" s="38">
+        <f t="shared" si="21"/>
+        <v>26.7776</v>
+      </c>
+      <c r="R75" s="36">
+        <v>10.38</v>
+      </c>
+      <c r="S75" s="42">
+        <f t="shared" si="19"/>
+        <v>8.1302727272727271</v>
+      </c>
+      <c r="T75" s="42">
+        <f t="shared" si="20"/>
+        <v>9.4902727272727265</v>
+      </c>
+      <c r="U75" s="43">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="76" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P76" s="43">
+        <v>10</v>
+      </c>
+      <c r="Q76" s="38">
+        <f t="shared" si="21"/>
+        <v>53.555199999999999</v>
+      </c>
+      <c r="R76" s="36">
+        <v>10.39</v>
+      </c>
+      <c r="S76" s="42">
+        <f t="shared" si="19"/>
+        <v>16.244696969696971</v>
+      </c>
+      <c r="T76" s="42">
+        <f t="shared" si="20"/>
+        <v>17.60469696969697</v>
+      </c>
+      <c r="U76" s="43">
+        <v>6.74</v>
       </c>
     </row>
   </sheetData>
@@ -19160,15 +20715,15 @@
         <v>0</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="44"/>
+      <c r="E2" s="49"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="44"/>
+      <c r="H2" s="49"/>
       <c r="I2" s="6"/>
       <c r="L2" s="3" t="s">
         <v>26</v>
@@ -20167,105 +21722,363 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:Z14"/>
+  <dimension ref="A2:Z18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B2" sqref="B2:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="2" max="2" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="26" width="9.140625" style="3"/>
+    <col min="5" max="5" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="8" max="26" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>125</v>
+      </c>
+      <c r="C4" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D4" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="E4" s="47">
+        <v>1</v>
+      </c>
+      <c r="F4" s="47">
+        <v>0</v>
+      </c>
+      <c r="G4" s="47">
+        <f>-10*LOG10(1+(2*PI()*B4*100000*47*10^-12)^2)</f>
+        <v>-5.917752955845818E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
         <v>250</v>
       </c>
+      <c r="C5" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D5" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="E5" s="47">
+        <v>1</v>
+      </c>
+      <c r="F5" s="47">
+        <v>0</v>
+      </c>
+      <c r="G5" s="47">
+        <f t="shared" ref="G5:G18" si="0">-10*LOG10(1+(2*PI()*B5*100000*47*10^-12)^2)</f>
+        <v>-2.3670528022348052E-4</v>
+      </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="3">
-        <f>C3*2</f>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
         <v>500</v>
       </c>
+      <c r="C6" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D6" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="E6" s="47">
+        <v>1</v>
+      </c>
+      <c r="F6" s="47">
+        <v>0</v>
+      </c>
+      <c r="G6" s="47">
+        <f t="shared" si="0"/>
+        <v>-9.4674372327238328E-4</v>
+      </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="3">
-        <f t="shared" ref="C5:C14" si="0">C4*2</f>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
         <v>1000</v>
       </c>
+      <c r="C7" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D7" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="E7" s="47">
+        <v>1</v>
+      </c>
+      <c r="F7" s="47">
+        <v>0</v>
+      </c>
+      <c r="G7" s="47">
+        <f t="shared" si="0"/>
+        <v>-3.7857372056880638E-3</v>
+      </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>2000</v>
+      </c>
+      <c r="C8" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D8" s="47">
+        <v>1.39</v>
+      </c>
+      <c r="E8" s="47">
+        <v>0.98581560300000004</v>
+      </c>
+      <c r="F8" s="47">
+        <v>-0.124086248</v>
+      </c>
+      <c r="G8" s="47">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>-1.5123188882178356E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>4000</v>
+      </c>
+      <c r="C9" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D9" s="47">
+        <v>1.39</v>
+      </c>
+      <c r="E9" s="47">
+        <v>0.98581560300000004</v>
+      </c>
+      <c r="F9" s="47">
+        <v>-0.124086248</v>
+      </c>
+      <c r="G9" s="47">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>-6.0179324114907472E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>8000</v>
+      </c>
+      <c r="C10" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D10" s="47">
+        <v>1.39</v>
+      </c>
+      <c r="E10" s="47">
+        <v>0.98581560300000004</v>
+      </c>
+      <c r="F10" s="47">
+        <v>-0.124086248</v>
+      </c>
+      <c r="G10" s="47">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>-0.23587008228984918</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>16000</v>
+      </c>
+      <c r="C11" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D11" s="47">
+        <v>1.26</v>
+      </c>
+      <c r="E11" s="47">
+        <v>0.89361702099999996</v>
+      </c>
+      <c r="F11" s="47">
+        <v>-0.97697135099999999</v>
+      </c>
+      <c r="G11" s="47">
         <f t="shared" si="0"/>
-        <v>16000</v>
+        <v>-0.87515945393713102</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>32000</v>
+      </c>
+      <c r="C12" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D12" s="47">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="E12" s="47">
+        <v>0.68226950399999997</v>
+      </c>
+      <c r="F12" s="47">
+        <v>-3.320880812</v>
+      </c>
+      <c r="G12" s="47">
         <f t="shared" si="0"/>
-        <v>32000</v>
+        <v>-2.7715247749318932</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>64000</v>
+      </c>
+      <c r="C13" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D13" s="47">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="E13" s="47">
+        <v>0.41773049600000001</v>
+      </c>
+      <c r="F13" s="47">
+        <v>-7.582076357</v>
+      </c>
+      <c r="G13" s="47">
         <f t="shared" si="0"/>
-        <v>64000</v>
+        <v>-6.6010930803660717</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>128000</v>
+      </c>
+      <c r="C14" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D14" s="47">
+        <v>0.314</v>
+      </c>
+      <c r="E14" s="47">
+        <v>0.22269503500000001</v>
+      </c>
+      <c r="F14" s="47">
+        <v>-13.04578929</v>
+      </c>
+      <c r="G14" s="47">
         <f t="shared" si="0"/>
-        <v>128000</v>
+        <v>-11.843543659922357</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>256000</v>
+      </c>
+      <c r="C15" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D15" s="47">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="E15" s="47">
+        <v>0.116312057</v>
+      </c>
+      <c r="F15" s="47">
+        <v>-18.687505290000001</v>
+      </c>
+      <c r="G15" s="47">
         <f t="shared" si="0"/>
-        <v>256000</v>
+        <v>-17.645685382570811</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>512000</v>
+      </c>
+      <c r="C16" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D16" s="47">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="E16" s="47">
+        <v>6.7375886999999995E-2</v>
+      </c>
+      <c r="F16" s="47">
+        <v>-23.429910150000001</v>
+      </c>
+      <c r="G16" s="47">
         <f t="shared" si="0"/>
-        <v>512000</v>
+        <v>-23.609909488085265</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="C17" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D17" s="47">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="E17" s="47">
+        <v>4.0425532E-2</v>
+      </c>
+      <c r="F17" s="47">
+        <v>-27.866885140000001</v>
+      </c>
+      <c r="G17" s="47">
+        <f t="shared" si="0"/>
+        <v>-29.410531667261782</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>2000000</v>
+      </c>
+      <c r="C18" s="47">
+        <v>1.41</v>
+      </c>
+      <c r="D18" s="47">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E18" s="47">
+        <v>3.8297871999999997E-2</v>
+      </c>
+      <c r="F18" s="47">
+        <v>-28.336507059999999</v>
+      </c>
+      <c r="G18" s="47">
+        <f t="shared" si="0"/>
+        <v>-35.427399259349919</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -20523,43 +22336,43 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="14"/>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="17"/>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="18"/>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="19"/>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
finished ch06 and added appendix
</commit_message>
<xml_diff>
--- a/Elaborato Scritto/data/Misure VCO Tesi.xlsx
+++ b/Elaborato Scritto/data/Misure VCO Tesi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\_PROGETTI\PRJ_SYNTH_MODULES\FG-VCO\Elaborato Scritto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53390812-45E0-4302-A879-A7AA49EBDC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63755200-B4DA-43CE-8B1C-DDED94267B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-690" yWindow="795" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="795" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Misure VFC110" sheetId="5" r:id="rId1"/>
@@ -4392,49 +4392,49 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-5.917752955845818E-5</c:v>
+                  <c:v>-2.4110453429220479E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.3670528022348052E-4</c:v>
+                  <c:v>-9.6441010614292289E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-9.4674372327238328E-4</c:v>
+                  <c:v>-3.857511934972326E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.7857372056880638E-3</c:v>
+                  <c:v>-1.5427992362868456E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.5123188882178356E-2</c:v>
+                  <c:v>-6.167911259831617E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-6.0179324114907472E-2</c:v>
+                  <c:v>-2.4619260041664114E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.23587008228984918</c:v>
+                  <c:v>-9.7650585946871399E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.87515945393713102</c:v>
+                  <c:v>-0.37808140461474932</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.7715247749318932</c:v>
+                  <c:v>-1.3476122542118065</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-6.6010930803660717</c:v>
+                  <c:v>-3.9011029233705701</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-11.843543659922357</c:v>
+                  <c:v>-8.3386903130340659</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-17.645685382570811</c:v>
+                  <c:v>-13.85343797951775</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-23.609909488085265</c:v>
+                  <c:v>-19.737800654423079</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-29.410531667261782</c:v>
+                  <c:v>-25.518228412625152</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-35.427399259349919</c:v>
+                  <c:v>-31.529677080213766</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5959,7 +5959,7 @@
             <c:numRef>
               <c:f>'Misure VCO'!$U$6:$U$17</c:f>
               <c:numCache>
-                <c:formatCode>0,000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>3.9600000000000003E-2</c:v>
@@ -18346,7 +18346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
@@ -21724,8 +21724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:Z18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21777,8 +21777,8 @@
         <v>0</v>
       </c>
       <c r="G4" s="47">
-        <f>-10*LOG10(1+(2*PI()*B4*100000*47*10^-12)^2)</f>
-        <v>-5.917752955845818E-5</v>
+        <f>-10*LOG10(1+(2*PI()*B4*100000*30*10^-12)^2)</f>
+        <v>-2.4110453429220479E-5</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -21798,8 +21798,8 @@
         <v>0</v>
       </c>
       <c r="G5" s="47">
-        <f t="shared" ref="G5:G18" si="0">-10*LOG10(1+(2*PI()*B5*100000*47*10^-12)^2)</f>
-        <v>-2.3670528022348052E-4</v>
+        <f t="shared" ref="G5:G18" si="0">-10*LOG10(1+(2*PI()*B5*100000*30*10^-12)^2)</f>
+        <v>-9.6441010614292289E-5</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -21820,7 +21820,7 @@
       </c>
       <c r="G6" s="47">
         <f t="shared" si="0"/>
-        <v>-9.4674372327238328E-4</v>
+        <v>-3.857511934972326E-4</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -21841,7 +21841,7 @@
       </c>
       <c r="G7" s="47">
         <f t="shared" si="0"/>
-        <v>-3.7857372056880638E-3</v>
+        <v>-1.5427992362868456E-3</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -21862,7 +21862,7 @@
       </c>
       <c r="G8" s="47">
         <f t="shared" si="0"/>
-        <v>-1.5123188882178356E-2</v>
+        <v>-6.167911259831617E-3</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -21883,7 +21883,7 @@
       </c>
       <c r="G9" s="47">
         <f t="shared" si="0"/>
-        <v>-6.0179324114907472E-2</v>
+        <v>-2.4619260041664114E-2</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -21904,7 +21904,7 @@
       </c>
       <c r="G10" s="47">
         <f t="shared" si="0"/>
-        <v>-0.23587008228984918</v>
+        <v>-9.7650585946871399E-2</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -21925,7 +21925,7 @@
       </c>
       <c r="G11" s="47">
         <f t="shared" si="0"/>
-        <v>-0.87515945393713102</v>
+        <v>-0.37808140461474932</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -21946,7 +21946,7 @@
       </c>
       <c r="G12" s="47">
         <f t="shared" si="0"/>
-        <v>-2.7715247749318932</v>
+        <v>-1.3476122542118065</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -21967,7 +21967,7 @@
       </c>
       <c r="G13" s="47">
         <f t="shared" si="0"/>
-        <v>-6.6010930803660717</v>
+        <v>-3.9011029233705701</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -21988,7 +21988,7 @@
       </c>
       <c r="G14" s="47">
         <f t="shared" si="0"/>
-        <v>-11.843543659922357</v>
+        <v>-8.3386903130340659</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -22009,7 +22009,7 @@
       </c>
       <c r="G15" s="47">
         <f t="shared" si="0"/>
-        <v>-17.645685382570811</v>
+        <v>-13.85343797951775</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
@@ -22030,7 +22030,7 @@
       </c>
       <c r="G16" s="47">
         <f t="shared" si="0"/>
-        <v>-23.609909488085265</v>
+        <v>-19.737800654423079</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -22051,7 +22051,7 @@
       </c>
       <c r="G17" s="47">
         <f t="shared" si="0"/>
-        <v>-29.410531667261782</v>
+        <v>-25.518228412625152</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -22072,7 +22072,7 @@
       </c>
       <c r="G18" s="47">
         <f t="shared" si="0"/>
-        <v>-35.427399259349919</v>
+        <v>-31.529677080213766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>